<commit_message>
river update May 2024
</commit_message>
<xml_diff>
--- a/data/Rivers/ManganuioteAoatAshworth_40125c59aa.xlsx
+++ b/data/Rivers/ManganuioteAoatAshworth_40125c59aa.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I41"/>
+  <dimension ref="A1:I44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1564,6 +1564,87 @@
       </c>
       <c r="I41" t="inlineStr"/>
     </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Manganui o te Ao at Ashworth</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>ASPM (Macroinvertebrate Average Score Per Metric)</t>
+        </is>
+      </c>
+      <c r="C42" s="2" t="n">
+        <v>45021</v>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>0.391</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr"/>
+      <c r="F42" t="inlineStr"/>
+      <c r="G42" t="inlineStr"/>
+      <c r="H42" t="n">
+        <v>200</v>
+      </c>
+      <c r="I42" t="inlineStr"/>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Manganui o te Ao at Ashworth</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>MCI (Macroinvertebrate Community Index)</t>
+        </is>
+      </c>
+      <c r="C43" s="2" t="n">
+        <v>45021</v>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>104.76</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr"/>
+      <c r="F43" t="inlineStr"/>
+      <c r="G43" t="inlineStr"/>
+      <c r="H43" t="n">
+        <v>200</v>
+      </c>
+      <c r="I43" t="inlineStr"/>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Manganui o te Ao at Ashworth</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>QMCI (Quantitative Macroinvertebrate Community Index)</t>
+        </is>
+      </c>
+      <c r="C44" s="2" t="n">
+        <v>45021</v>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>4.079</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr"/>
+      <c r="F44" t="inlineStr"/>
+      <c r="G44" t="inlineStr"/>
+      <c r="H44" t="n">
+        <v>200</v>
+      </c>
+      <c r="I44" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>